<commit_message>
AzureAD master application and setDataFromDataExcel
</commit_message>
<xml_diff>
--- a/src/main/resources/input/inputExcel.xlsx
+++ b/src/main/resources/input/inputExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Documents\2ºDAM\TFG\Proyects\META-2\src\main\resources\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92979421-62D7-40B7-A131-68B227FE3161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98873E10-ACB6-4607-B4A9-0698A470C786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AZUREAD" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>SCOPE</t>
   </si>
@@ -58,6 +58,27 @@
   </si>
   <si>
     <t>VPNs</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>CLIENT ID</t>
+  </si>
+  <si>
+    <t>CLIENT SECRET</t>
+  </si>
+  <si>
+    <t>Irisrusk</t>
+  </si>
+  <si>
+    <t>CLIENTID</t>
+  </si>
+  <si>
+    <t>CLIENTSECRET</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -129,12 +150,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E426E149-A91F-4D02-9CDC-FDC46EFB4B8A}" name="Tabla1" displayName="Tabla1" ref="A1:C4" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:C4" xr:uid="{E426E149-A91F-4D02-9CDC-FDC46EFB4B8A}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E426E149-A91F-4D02-9CDC-FDC46EFB4B8A}" name="Tabla1" displayName="Tabla1" ref="A1:F4" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:F4" xr:uid="{E426E149-A91F-4D02-9CDC-FDC46EFB4B8A}"/>
+  <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{F33831BB-F014-4E30-A6B9-B1BEDAFB4D48}" name="TYPE"/>
     <tableColumn id="1" xr3:uid="{3D6CC73F-9521-4077-82D1-ADB25080F9B6}" name="SCOPE"/>
     <tableColumn id="2" xr3:uid="{8F46D3F0-FAD2-498C-A186-EEAD24937312}" name="APP NAME"/>
+    <tableColumn id="3" xr3:uid="{4C933D40-BC16-4340-B47B-4C15AC703448}" name="URL"/>
+    <tableColumn id="5" xr3:uid="{54907F5D-C55A-462F-8F86-4FD1AB4C0617}" name="CLIENT ID"/>
+    <tableColumn id="6" xr3:uid="{5A4BEEB0-6964-4E15-9EC9-E35467B12441}" name="CLIENT SECRET"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -415,19 +439,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="4" max="6" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -437,8 +461,17 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -448,8 +481,17 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -458,6 +500,35 @@
       </c>
       <c r="C3" t="s">
         <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -474,7 +545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AC30E3F-C42A-4365-96A6-D5220C04BA3D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>